<commit_message>
sector figures growth rate fix
</commit_message>
<xml_diff>
--- a/Results/Public data/ipcc_ar6_data_growth_rates.xlsx
+++ b/Results/Public data/ipcc_ar6_data_growth_rates.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Last update</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-08-16 13:24:16</t>
+    <t xml:space="preserve">2021-08-16 13:35:49</t>
   </si>
   <si>
     <t xml:space="preserve">Code</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">important note</t>
   </si>
   <si>
-    <t xml:space="preserve">Growth rates include the first and last year. For example, the estimate for 1990-2000 has 11 years of data. Also, some years (e.g. 2000) have a leap year adjustment applied to them, so will show slightly different totals.</t>
+    <t xml:space="preserve">Growth rates assume emissions are at the end of each year - 31.12. For example, the estimate for 1990-2000 has 10 years of data.</t>
   </si>
   <si>
     <t xml:space="preserve">category</t>

</xml_diff>

<commit_message>
add land to growth rate
</commit_message>
<xml_diff>
--- a/Results/Public data/ipcc_ar6_data_growth_rates.xlsx
+++ b/Results/Public data/ipcc_ar6_data_growth_rates.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="318">
   <si>
     <t xml:space="preserve">Author</t>
   </si>
@@ -29,7 +29,7 @@
     <t xml:space="preserve">Last update</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-08-24 15:19:11</t>
+    <t xml:space="preserve">2021-08-25 11:29:46</t>
   </si>
   <si>
     <t xml:space="preserve">Code</t>
@@ -119,19 +119,22 @@
     <t xml:space="preserve">Gases</t>
   </si>
   <si>
+    <t xml:space="preserve">CO2_FFI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2_LULUCF</t>
+  </si>
+  <si>
     <t xml:space="preserve">CH4</t>
   </si>
   <si>
-    <t xml:space="preserve">CO2</t>
+    <t xml:space="preserve">N2O</t>
   </si>
   <si>
     <t xml:space="preserve">Fgas</t>
   </si>
   <si>
     <t xml:space="preserve">GHG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2O</t>
   </si>
   <si>
     <t xml:space="preserve">Regions</t>
@@ -1454,28 +1457,28 @@
         <v>33</v>
       </c>
       <c r="D2" t="n">
-        <v>8.17558268994896</v>
+        <v>22.7048976097961</v>
       </c>
       <c r="E2" t="n">
-        <v>8.43768841872268</v>
+        <v>25.8123841524056</v>
       </c>
       <c r="F2" t="n">
-        <v>9.66424928526536</v>
+        <v>34.1369545479154</v>
       </c>
       <c r="G2" t="n">
-        <v>10.565894553494</v>
+        <v>37.9300547752771</v>
       </c>
       <c r="H2" t="n">
-        <v>0.316062384764004</v>
+        <v>1.29099964213424</v>
       </c>
       <c r="I2" t="n">
-        <v>1.36650294724756</v>
+        <v>2.83469525693971</v>
       </c>
       <c r="J2" t="n">
-        <v>0.996015124879857</v>
+        <v>1.1775827864235</v>
       </c>
       <c r="K2" t="n">
-        <v>0.888333947826836</v>
+        <v>1.78527699058815</v>
       </c>
     </row>
     <row r="3">
@@ -1487,28 +1490,28 @@
         <v>34</v>
       </c>
       <c r="D3" t="n">
-        <v>22.7048976097961</v>
+        <v>4.979180807728</v>
       </c>
       <c r="E3" t="n">
-        <v>25.8123841524056</v>
+        <v>5.05170398532267</v>
       </c>
       <c r="F3" t="n">
-        <v>34.1369545479154</v>
+        <v>5.33731686335467</v>
       </c>
       <c r="G3" t="n">
-        <v>37.9300547752771</v>
+        <v>6.6050388476</v>
       </c>
       <c r="H3" t="n">
-        <v>1.29099964213424</v>
+        <v>0.144706880948475</v>
       </c>
       <c r="I3" t="n">
-        <v>2.83469525693971</v>
+        <v>0.551489710927444</v>
       </c>
       <c r="J3" t="n">
-        <v>1.1775827864235</v>
+        <v>2.3961431572314</v>
       </c>
       <c r="K3" t="n">
-        <v>1.78527699058815</v>
+        <v>0.979132921884363</v>
       </c>
     </row>
     <row r="4">
@@ -1520,28 +1523,28 @@
         <v>35</v>
       </c>
       <c r="D4" t="n">
-        <v>0.286439531994979</v>
+        <v>8.17558268994896</v>
       </c>
       <c r="E4" t="n">
-        <v>0.524520427692494</v>
+        <v>8.43768841872268</v>
       </c>
       <c r="F4" t="n">
-        <v>0.657571963830359</v>
+        <v>9.66424928526536</v>
       </c>
       <c r="G4" t="n">
-        <v>0.692236336011965</v>
+        <v>10.565894553494</v>
       </c>
       <c r="H4" t="n">
-        <v>6.23630206658874</v>
+        <v>0.316062384764004</v>
       </c>
       <c r="I4" t="n">
-        <v>2.28644578995516</v>
+        <v>1.36650294724756</v>
       </c>
       <c r="J4" t="n">
-        <v>0.572445739829575</v>
+        <v>0.996015124879857</v>
       </c>
       <c r="K4" t="n">
-        <v>3.08952351408778</v>
+        <v>0.888333947826836</v>
       </c>
     </row>
     <row r="5">
@@ -1553,28 +1556,28 @@
         <v>36</v>
       </c>
       <c r="D5" t="n">
-        <v>33.0651873586009</v>
+        <v>1.89826752686084</v>
       </c>
       <c r="E5" t="n">
-        <v>36.8106441151285</v>
+        <v>2.03605111630764</v>
       </c>
       <c r="F5" t="n">
-        <v>46.7296637448991</v>
+        <v>2.27088794788791</v>
       </c>
       <c r="G5" t="n">
-        <v>51.7208634023013</v>
+        <v>2.53267773751827</v>
       </c>
       <c r="H5" t="n">
-        <v>1.07883852479069</v>
+        <v>0.703166309668291</v>
       </c>
       <c r="I5" t="n">
-        <v>2.41461197824893</v>
+        <v>1.09756671889707</v>
       </c>
       <c r="J5" t="n">
-        <v>1.13395987014779</v>
+        <v>1.21966932213784</v>
       </c>
       <c r="K5" t="n">
-        <v>1.55465145002682</v>
+        <v>0.999219517967798</v>
       </c>
     </row>
     <row r="6">
@@ -1586,28 +1589,61 @@
         <v>37</v>
       </c>
       <c r="D6" t="n">
-        <v>1.89826752686084</v>
+        <v>0.286439531994979</v>
       </c>
       <c r="E6" t="n">
-        <v>2.03605111630764</v>
+        <v>0.524520427692494</v>
       </c>
       <c r="F6" t="n">
-        <v>2.27088794788791</v>
+        <v>0.657571963830359</v>
       </c>
       <c r="G6" t="n">
-        <v>2.53267773751827</v>
+        <v>0.692236336011965</v>
       </c>
       <c r="H6" t="n">
-        <v>0.703166309668291</v>
+        <v>6.23630206658874</v>
       </c>
       <c r="I6" t="n">
-        <v>1.09756671889707</v>
+        <v>2.28644578995516</v>
       </c>
       <c r="J6" t="n">
-        <v>1.21966932213784</v>
+        <v>0.572445739829575</v>
       </c>
       <c r="K6" t="n">
-        <v>0.999219517967798</v>
+        <v>3.08952351408778</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="n">
+        <v>38.0443681663289</v>
+      </c>
+      <c r="E7" t="n">
+        <v>41.8623481004511</v>
+      </c>
+      <c r="F7" t="n">
+        <v>52.0669806082537</v>
+      </c>
+      <c r="G7" t="n">
+        <v>58.3259022499013</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.960924995466983</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2.20540908767668</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.26926890757961</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.48433332923716</v>
       </c>
     </row>
   </sheetData>
@@ -1661,13 +1697,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" t="n">
         <v>2.77742968905457</v>
@@ -1696,13 +1732,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D3" t="n">
         <v>9.77017545921387</v>
@@ -1731,13 +1767,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" t="n">
         <v>15.7002495055422</v>
@@ -1766,13 +1802,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D5" t="n">
         <v>4.31504112845735</v>
@@ -1801,13 +1837,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" t="n">
         <v>0.261952849520111</v>
@@ -1836,13 +1872,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" t="n">
         <v>0.395632549408763</v>
@@ -1871,13 +1907,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D8" t="n">
         <v>3.7113472028784</v>
@@ -1906,13 +1942,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" t="n">
         <v>1.11253978225356</v>
@@ -1990,11 +2026,11 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2"/>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
         <v>10.2006329267325</v>
@@ -2023,11 +2059,11 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" t="n">
         <v>3.00366446455348</v>
@@ -2056,11 +2092,11 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" t="n">
         <v>11.961001787345</v>
@@ -2089,11 +2125,11 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" t="n">
         <v>7.8535323725065</v>
@@ -2122,11 +2158,11 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6"/>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" t="n">
         <v>5.02553661519145</v>
@@ -2204,11 +2240,11 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2"/>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
         <v>10.2006329267325</v>
@@ -2237,11 +2273,11 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" t="n">
         <v>6.37968410340929</v>
@@ -2264,11 +2300,11 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" t="n">
         <v>11.961001787345</v>
@@ -2297,11 +2333,11 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" t="n">
         <v>11.2702223900935</v>
@@ -2324,11 +2360,11 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6"/>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" t="n">
         <v>5.11414289499238</v>
@@ -2400,13 +2436,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2" t="n">
         <v>41.7228438687474</v>
@@ -2435,13 +2471,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D3" t="n">
         <v>2459.33548371225</v>
@@ -2470,13 +2506,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D4" t="n">
         <v>1057.59672099974</v>
@@ -2505,13 +2541,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D5" t="n">
         <v>383.572847364061</v>
@@ -2540,13 +2576,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D6" t="n">
         <v>1055.34627839291</v>
@@ -2575,13 +2611,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D7" t="n">
         <v>223.87794466674</v>
@@ -2610,13 +2646,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D8" t="n">
         <v>0.0096074973</v>
@@ -2645,13 +2681,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D9" t="n">
         <v>782.237072260382</v>
@@ -2680,13 +2716,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D10" t="n">
         <v>2221.4177847958</v>
@@ -2715,13 +2751,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D11" t="n">
         <v>95.9186328307005</v>
@@ -2750,13 +2786,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12" t="n">
         <v>910.445857038311</v>
@@ -2785,13 +2821,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D13" t="n">
         <v>7655.34107363202</v>
@@ -2820,13 +2856,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D14" t="n">
         <v>1766.95843965939</v>
@@ -2855,13 +2891,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D15" t="n">
         <v>1003.19629466337</v>
@@ -2890,13 +2926,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D16" t="n">
         <v>529.141489521187</v>
@@ -2925,13 +2961,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D17" t="n">
         <v>514.67258857</v>
@@ -2960,13 +2996,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D18" t="n">
         <v>1658.7650952988</v>
@@ -2995,13 +3031,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D19" t="n">
         <v>1550.63095474604</v>
@@ -3030,13 +3066,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D20" t="n">
         <v>2562.6738631167</v>
@@ -3065,13 +3101,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D21" t="n">
         <v>1566.78987077497</v>
@@ -3100,13 +3136,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D22" t="n">
         <v>286.86437717727</v>
@@ -3135,13 +3171,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D23" t="n">
         <v>101.31055182816</v>
@@ -3170,13 +3206,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D24" t="n">
         <v>260.335372841111</v>
@@ -3205,13 +3241,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D25" t="n">
         <v>374.833673104063</v>
@@ -3240,13 +3276,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D26" t="n">
         <v>481.055667363867</v>
@@ -3275,13 +3311,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D27" t="n">
         <v>137.791616844951</v>
@@ -3310,13 +3346,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D28" t="n">
         <v>3383.34535603202</v>
@@ -3394,13 +3430,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" t="n">
         <v>145.787605584505</v>
@@ -3429,13 +3465,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D3" t="n">
         <v>33.6524949546942</v>
@@ -3464,13 +3500,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D4" t="n">
         <v>4.01139690278578</v>
@@ -3499,13 +3535,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" t="n">
         <v>8.92938037062645</v>
@@ -3534,13 +3570,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D6" t="n">
         <v>10.6061764000469</v>
@@ -3569,13 +3605,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D7" t="n">
         <v>2.90561338084759</v>
@@ -3604,13 +3640,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D8" t="n">
         <v>0.225977910859409</v>
@@ -3639,13 +3675,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D9" t="n">
         <v>30.5958289667847</v>
@@ -3674,13 +3710,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D10" t="n">
         <v>4.90771059278994</v>
@@ -3709,13 +3745,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D11" t="n">
         <v>10.3492282256256</v>
@@ -3744,13 +3780,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D12" t="n">
         <v>0.328025198782607</v>
@@ -3779,13 +3815,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D13" t="n">
         <v>24.7141146750246</v>
@@ -3814,13 +3850,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D14" t="n">
         <v>11.1867514051475</v>
@@ -3849,13 +3885,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D15" t="n">
         <v>10.6146213959633</v>
@@ -3884,13 +3920,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D16" t="n">
         <v>2.04795362870598</v>
@@ -3919,13 +3955,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D17" t="n">
         <v>147.350491536952</v>
@@ -3954,13 +3990,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D18" t="n">
         <v>0.223413949001943</v>
@@ -3989,13 +4025,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D19" t="n">
         <v>4.66155427123775</v>
@@ -4024,13 +4060,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D20" t="n">
         <v>65.2420895679627</v>
@@ -4059,13 +4095,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -4094,13 +4130,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D22" t="n">
         <v>20.2282038741512</v>
@@ -4129,13 +4165,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D23" t="n">
         <v>0.935378751805203</v>
@@ -4164,13 +4200,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D24" t="n">
         <v>10.7805594997052</v>
@@ -4199,13 +4235,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D25" t="n">
         <v>7.32319810660677</v>
@@ -4234,13 +4270,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D26" t="n">
         <v>1.57434149852513</v>
@@ -4269,13 +4305,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D27" t="n">
         <v>41.2708457104508</v>
@@ -4304,13 +4340,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D28" t="n">
         <v>2.04614989282007</v>
@@ -4339,13 +4375,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D29" t="n">
         <v>1.64215800567868</v>
@@ -4374,13 +4410,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D30" t="n">
         <v>90.6550471876566</v>
@@ -4409,13 +4445,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D31" t="n">
         <v>24.5301915152394</v>
@@ -4444,13 +4480,13 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D32" t="n">
         <v>5.10152920281963</v>
@@ -4479,13 +4515,13 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D33" t="n">
         <v>12.7953243482818</v>
@@ -4514,13 +4550,13 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D34" t="n">
         <v>6.45228318668787</v>
@@ -4549,13 +4585,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D35" t="n">
         <v>1.92757364977348</v>
@@ -4584,13 +4620,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D36" t="n">
         <v>0.011897119809</v>
@@ -4619,13 +4655,13 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D37" t="n">
         <v>44.0745999658707</v>
@@ -4654,13 +4690,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D38" t="n">
         <v>8.216692331718</v>
@@ -4689,13 +4725,13 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D39" t="n">
         <v>6.95093414859749</v>
@@ -4724,13 +4760,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D40" t="n">
         <v>12.1711584212029</v>
@@ -4759,13 +4795,13 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D41" t="n">
         <v>283.970625411488</v>
@@ -4794,13 +4830,13 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D42" t="n">
         <v>1.22314536642967</v>
@@ -4829,13 +4865,13 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D43" t="n">
         <v>3.68729835650379</v>
@@ -4864,13 +4900,13 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D44" t="n">
         <v>0.0136672062023045</v>
@@ -4899,13 +4935,13 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D45" t="n">
         <v>0.0859095622512935</v>
@@ -4934,13 +4970,13 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D46" t="n">
         <v>9.95699507361876</v>
@@ -4969,13 +5005,13 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D47" t="n">
         <v>0.367867231637188</v>
@@ -5004,13 +5040,13 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D48" t="n">
         <v>3.86244861227275</v>
@@ -5039,13 +5075,13 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C49" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D49" t="n">
         <v>24.6168697467781</v>
@@ -5074,13 +5110,13 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D50" t="n">
         <v>402.637340408586</v>
@@ -5109,13 +5145,13 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D51" t="n">
         <v>58.6735601970659</v>
@@ -5144,13 +5180,13 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D52" t="n">
         <v>2.86090414697794</v>
@@ -5179,13 +5215,13 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D53" t="n">
         <v>31.0738026901291</v>
@@ -5214,13 +5250,13 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C54" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D54" t="n">
         <v>3.37499776172939</v>
@@ -5249,13 +5285,13 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D55" t="n">
         <v>23.6829237302918</v>
@@ -5284,13 +5320,13 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D56" t="n">
         <v>16.0641004010505</v>
@@ -5319,13 +5355,13 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C57" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D57" t="n">
         <v>0.411582141033177</v>
@@ -5354,13 +5390,13 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D58" t="n">
         <v>15.406002555413</v>
@@ -5389,13 +5425,13 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C59" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D59" t="n">
         <v>34.4976821380344</v>
@@ -5424,13 +5460,13 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C60" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D60" t="n">
         <v>13.3644098337721</v>
@@ -5459,13 +5495,13 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C61" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D61" t="n">
         <v>0.0134917751416702</v>
@@ -5494,13 +5530,13 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C62" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D62" t="n">
         <v>135.572522940203</v>
@@ -5529,13 +5565,13 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C63" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D63" t="n">
         <v>1.11843072462214</v>
@@ -5564,13 +5600,13 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D64" t="n">
         <v>8.18368814236418</v>
@@ -5599,13 +5635,13 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B65" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C65" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D65" t="n">
         <v>19.3682360945501</v>
@@ -5634,13 +5670,13 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D66" t="n">
         <v>3893.72266167551</v>
@@ -5669,13 +5705,13 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D67" t="n">
         <v>0.0494723033925397</v>
@@ -5704,13 +5740,13 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C68" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D68" t="n">
         <v>2.14118044152554</v>
@@ -5739,13 +5775,13 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C69" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D69" t="n">
         <v>0.923785915209981</v>
@@ -5774,13 +5810,13 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C70" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D70" t="n">
         <v>0.047843045084096</v>
@@ -5809,13 +5845,13 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C71" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D71" t="n">
         <v>38.3285648197683</v>
@@ -5844,13 +5880,13 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C72" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D72" t="n">
         <v>1405.48350224253</v>
@@ -5879,13 +5915,13 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B73" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C73" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D73" t="n">
         <v>422.788557645902</v>
@@ -5914,13 +5950,13 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C74" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D74" t="n">
         <v>0.0337991593777183</v>
@@ -5949,13 +5985,13 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B75" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C75" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D75" t="n">
         <v>167.578079313218</v>
@@ -5984,13 +6020,13 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C76" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D76" t="n">
         <v>323.817568756721</v>
@@ -6019,13 +6055,13 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B77" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C77" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D77" t="n">
         <v>8.04292570247595</v>
@@ -6054,13 +6090,13 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B78" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C78" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D78" t="n">
         <v>1.01251589868371</v>
@@ -6089,13 +6125,13 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B79" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C79" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D79" t="n">
         <v>94.9797221024638</v>
@@ -6124,13 +6160,13 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B80" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C80" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D80" t="n">
         <v>0.144526604009972</v>
@@ -6159,13 +6195,13 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C81" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D81" t="n">
         <v>0.001874792357244</v>
@@ -6194,13 +6230,13 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C82" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D82" t="n">
         <v>0.035467371513456</v>
@@ -6229,13 +6265,13 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C83" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D83" t="n">
         <v>25.765699911942</v>
@@ -6264,13 +6300,13 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C84" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D84" t="n">
         <v>70.2268130652394</v>
@@ -6299,13 +6335,13 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C85" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D85" t="n">
         <v>0.00221620997442</v>
@@ -6334,13 +6370,13 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C86" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D86" t="n">
         <v>30.6382367538894</v>
@@ -6369,13 +6405,13 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C87" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D87" t="n">
         <v>1.90361042516075</v>
@@ -6404,13 +6440,13 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B88" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C88" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D88" t="n">
         <v>0.0011585953471083</v>
@@ -6439,13 +6475,13 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C89" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D89" t="n">
         <v>0.001751416269696</v>
@@ -6474,13 +6510,13 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B90" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C90" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D90" t="n">
         <v>209.338281862503</v>
@@ -6509,13 +6545,13 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B91" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C91" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D91" t="n">
         <v>2.31930308198094</v>
@@ -6544,13 +6580,13 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B92" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C92" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D92" t="n">
         <v>3.44859711219519</v>
@@ -6579,13 +6615,13 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B93" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C93" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D93" t="n">
         <v>107.17818572429</v>
@@ -6614,13 +6650,13 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B94" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C94" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D94" t="n">
         <v>0</v>
@@ -6649,13 +6685,13 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B95" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C95" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D95" t="n">
         <v>0.289176467632854</v>
@@ -6684,13 +6720,13 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B96" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C96" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D96" t="n">
         <v>33.7926800263988</v>
@@ -6719,13 +6755,13 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B97" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C97" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D97" t="n">
         <v>0.265748924696949</v>
@@ -6754,13 +6790,13 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B98" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C98" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D98" t="n">
         <v>22.181502783963</v>
@@ -6789,13 +6825,13 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B99" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C99" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D99" t="n">
         <v>142.221103648932</v>
@@ -6824,13 +6860,13 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B100" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C100" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D100" t="n">
         <v>213.384899274346</v>
@@ -6859,13 +6895,13 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B101" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C101" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D101" t="n">
         <v>0.721001593394187</v>
@@ -6894,13 +6930,13 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B102" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C102" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D102" t="n">
         <v>0.00041901579495</v>
@@ -6929,13 +6965,13 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B103" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C103" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D103" t="n">
         <v>0.181671041193295</v>
@@ -6964,13 +7000,13 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B104" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C104" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D104" t="n">
         <v>0.0043963900454</v>
@@ -6999,13 +7035,13 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B105" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C105" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D105" t="n">
         <v>0</v>
@@ -7034,13 +7070,13 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B106" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C106" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D106" t="n">
         <v>0.479426782579361</v>
@@ -7069,13 +7105,13 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B107" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C107" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D107" t="n">
         <v>108.279358141029</v>
@@ -7104,13 +7140,13 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B108" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C108" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D108" t="n">
         <v>0.0093041766794118</v>
@@ -7139,13 +7175,13 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B109" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C109" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D109" t="n">
         <v>11.3656783356161</v>
@@ -7174,13 +7210,13 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B110" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C110" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D110" t="n">
         <v>456.893858973098</v>
@@ -7209,13 +7245,13 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B111" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C111" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D111" t="n">
         <v>82.3671736033895</v>
@@ -7244,13 +7280,13 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B112" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C112" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D112" t="n">
         <v>145.038624430234</v>
@@ -7279,13 +7315,13 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B113" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C113" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D113" t="n">
         <v>0.763502775218347</v>
@@ -7314,13 +7350,13 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B114" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C114" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D114" t="n">
         <v>32.1104653496557</v>
@@ -7349,13 +7385,13 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B115" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C115" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D115" t="n">
         <v>103.662305139385</v>
@@ -7384,13 +7420,13 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B116" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C116" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D116" t="n">
         <v>593.414349454796</v>
@@ -7419,13 +7455,13 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B117" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C117" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D117" t="n">
         <v>0</v>
@@ -7454,13 +7490,13 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B118" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C118" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D118" t="n">
         <v>0</v>
@@ -7489,13 +7525,13 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B119" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C119" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D119" t="n">
         <v>34.5951707183415</v>
@@ -7524,13 +7560,13 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B120" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C120" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D120" t="n">
         <v>5.31443888680323</v>
@@ -7559,13 +7595,13 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B121" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C121" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D121" t="n">
         <v>195.697074615084</v>
@@ -7594,13 +7630,13 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B122" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C122" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D122" t="n">
         <v>70.5344104040192</v>
@@ -7629,13 +7665,13 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B123" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C123" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D123" t="n">
         <v>41.1467551378005</v>
@@ -7664,13 +7700,13 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B124" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C124" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D124" t="n">
         <v>0.045263403158824</v>
@@ -7699,13 +7735,13 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B125" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C125" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D125" t="n">
         <v>84.143562574772</v>
@@ -7734,13 +7770,13 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B126" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C126" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D126" t="n">
         <v>544.114790125585</v>
@@ -7769,13 +7805,13 @@
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B127" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C127" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D127" t="n">
         <v>1238.62790947637</v>
@@ -7804,13 +7840,13 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B128" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C128" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D128" t="n">
         <v>0.1586652919957</v>
@@ -7839,13 +7875,13 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B129" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C129" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D129" t="n">
         <v>102.350654013311</v>
@@ -7874,13 +7910,13 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B130" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C130" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D130" t="n">
         <v>0.0673323343077</v>
@@ -7909,13 +7945,13 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B131" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C131" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D131" t="n">
         <v>0</v>
@@ -7944,13 +7980,13 @@
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B132" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C132" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D132" t="n">
         <v>96.806584607235</v>
@@ -7979,13 +8015,13 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B133" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C133" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D133" t="n">
         <v>4.54872834368089</v>
@@ -8014,13 +8050,13 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B134" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C134" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D134" t="n">
         <v>58.3610853302695</v>
@@ -8049,13 +8085,13 @@
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B135" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C135" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D135" t="n">
         <v>522.007433086054</v>
@@ -8084,13 +8120,13 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B136" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C136" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D136" t="n">
         <v>1314.66607689382</v>
@@ -8119,13 +8155,13 @@
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B137" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C137" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D137" t="n">
         <v>28.1619143636335</v>
@@ -8154,13 +8190,13 @@
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B138" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C138" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D138" t="n">
         <v>47.4721383382888</v>
@@ -8189,13 +8225,13 @@
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B139" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C139" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D139" t="n">
         <v>12.7216057523905</v>
@@ -8224,13 +8260,13 @@
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B140" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C140" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D140" t="n">
         <v>2.51613175666306</v>
@@ -8259,13 +8295,13 @@
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B141" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C141" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D141" t="n">
         <v>223.579026337231</v>
@@ -8294,13 +8330,13 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B142" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C142" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D142" t="n">
         <v>70.2084655434692</v>
@@ -8329,13 +8365,13 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B143" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C143" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D143" t="n">
         <v>0</v>
@@ -8364,13 +8400,13 @@
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B144" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C144" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D144" t="n">
         <v>64.1640173163853</v>
@@ -8399,13 +8435,13 @@
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B145" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C145" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D145" t="n">
         <v>523.422077654562</v>
@@ -8434,13 +8470,13 @@
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B146" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C146" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D146" t="n">
         <v>58.6786358369147</v>
@@ -8469,13 +8505,13 @@
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B147" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C147" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D147" t="n">
         <v>247.016830086757</v>
@@ -8504,13 +8540,13 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B148" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C148" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D148" t="n">
         <v>0.241938147768287</v>
@@ -8539,13 +8575,13 @@
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B149" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C149" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D149" t="n">
         <v>74.8034901201926</v>
@@ -8574,13 +8610,13 @@
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B150" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C150" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D150" t="n">
         <v>23.2942998877636</v>
@@ -8609,13 +8645,13 @@
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B151" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C151" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D151" t="n">
         <v>299.732489280343</v>
@@ -8644,13 +8680,13 @@
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B152" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C152" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D152" t="n">
         <v>79.9287674591305</v>
@@ -8679,13 +8715,13 @@
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B153" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C153" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D153" t="n">
         <v>54.9120119662568</v>
@@ -8714,13 +8750,13 @@
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B154" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C154" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D154" t="n">
         <v>222.768914788005</v>
@@ -8749,13 +8785,13 @@
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B155" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C155" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D155" t="n">
         <v>960.448486930477</v>
@@ -8784,13 +8820,13 @@
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B156" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C156" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D156" t="n">
         <v>782.186800286448</v>
@@ -8819,13 +8855,13 @@
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B157" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C157" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D157" t="n">
         <v>6232.9808200389</v>
@@ -8854,13 +8890,13 @@
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B158" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C158" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D158" t="n">
         <v>24.286637460377</v>
@@ -8889,13 +8925,13 @@
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B159" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C159" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D159" t="n">
         <v>69.7272477203554</v>
@@ -8924,13 +8960,13 @@
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B160" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C160" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D160" t="n">
         <v>140.820143906815</v>
@@ -8959,13 +8995,13 @@
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B161" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C161" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D161" t="n">
         <v>42.2379109379696</v>
@@ -8994,13 +9030,13 @@
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B162" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C162" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D162" t="n">
         <v>354.904142129699</v>
@@ -9029,13 +9065,13 @@
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B163" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C163" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D163" t="n">
         <v>34.0227429675899</v>
@@ -9064,13 +9100,13 @@
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B164" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C164" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D164" t="n">
         <v>14.2934258524021</v>
@@ -9099,13 +9135,13 @@
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B165" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C165" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D165" t="n">
         <v>37.7535400976309</v>
@@ -9134,13 +9170,13 @@
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B166" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C166" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D166" t="n">
         <v>3078.78334813895</v>
@@ -9169,13 +9205,13 @@
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B167" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C167" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D167" t="n">
         <v>85.804853152071</v>
@@ -9204,13 +9240,13 @@
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B168" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C168" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D168" t="n">
         <v>22.4731926477642</v>
@@ -9239,13 +9275,13 @@
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B169" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C169" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D169" t="n">
         <v>83.9080207576699</v>
@@ -9274,13 +9310,13 @@
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B170" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C170" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D170" t="n">
         <v>170.376931008046</v>
@@ -9309,13 +9345,13 @@
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B171" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C171" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D171" t="n">
         <v>261.952849520111</v>
@@ -9344,13 +9380,13 @@
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B172" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C172" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D172" t="n">
         <v>395.632549408763</v>
@@ -9379,13 +9415,13 @@
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B173" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C173" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D173" t="n">
         <v>0.00855499455582336</v>
@@ -9414,13 +9450,13 @@
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B174" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C174" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D174" t="n">
         <v>0.492158535159409</v>
@@ -9449,13 +9485,13 @@
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B175" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C175" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D175" t="n">
         <v>271.702407805923</v>
@@ -9484,13 +9520,13 @@
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B176" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C176" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D176" t="n">
         <v>0.553762368145376</v>
@@ -9519,13 +9555,13 @@
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B177" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C177" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D177" t="n">
         <v>3.01366377883297</v>
@@ -9554,13 +9590,13 @@
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B178" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C178" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D178" t="n">
         <v>1.58006607444628</v>
@@ -9589,13 +9625,13 @@
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B179" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C179" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D179" t="n">
         <v>0.632003571673807</v>
@@ -9624,13 +9660,13 @@
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B180" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C180" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D180" t="n">
         <v>30.8906101602765</v>
@@ -9659,13 +9695,13 @@
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B181" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C181" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D181" t="n">
         <v>0</v>
@@ -9694,13 +9730,13 @@
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B182" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C182" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D182" t="n">
         <v>696.13927129911</v>
@@ -9729,13 +9765,13 @@
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B183" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C183" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D183" t="n">
         <v>0.0572353637487174</v>
@@ -9764,13 +9800,13 @@
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B184" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C184" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D184" t="n">
         <v>0.298707899186892</v>
@@ -9799,13 +9835,13 @@
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B185" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C185" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D185" t="n">
         <v>58.4859784876316</v>
@@ -9834,13 +9870,13 @@
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B186" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C186" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D186" t="n">
         <v>135.171855877777</v>
@@ -9869,13 +9905,13 @@
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B187" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C187" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D187" t="n">
         <v>9.78164294572855</v>
@@ -9904,13 +9940,13 @@
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B188" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C188" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D188" t="n">
         <v>62.7161480180483</v>
@@ -9939,13 +9975,13 @@
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B189" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C189" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D189" t="n">
         <v>0.00211452416</v>
@@ -9974,13 +10010,13 @@
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B190" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C190" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D190" t="n">
         <v>0.112197815704147</v>
@@ -10009,13 +10045,13 @@
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B191" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C191" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D191" t="n">
         <v>17.6993847181369</v>
@@ -10044,13 +10080,13 @@
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B192" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C192" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D192" t="n">
         <v>38.0321795388891</v>
@@ -10079,13 +10115,13 @@
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B193" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C193" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D193" t="n">
         <v>7.65744574639809</v>
@@ -10114,13 +10150,13 @@
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B194" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C194" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D194" t="n">
         <v>0.174731343464394</v>
@@ -10149,13 +10185,13 @@
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B195" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C195" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D195" t="n">
         <v>0.744591978992194</v>
@@ -10184,13 +10220,13 @@
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B196" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C196" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D196" t="n">
         <v>0.170619484575769</v>
@@ -10219,13 +10255,13 @@
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B197" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C197" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D197" t="n">
         <v>1.79571809667106</v>
@@ -10254,13 +10290,13 @@
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B198" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C198" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D198" t="n">
         <v>13.7155115316782</v>
@@ -10289,13 +10325,13 @@
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B199" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C199" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D199" t="n">
         <v>3.09686699582799</v>
@@ -10324,13 +10360,13 @@
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B200" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C200" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D200" t="n">
         <v>6.18942904997111</v>
@@ -10359,13 +10395,13 @@
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B201" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C201" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D201" t="n">
         <v>9.49966589024035</v>
@@ -10394,13 +10430,13 @@
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B202" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C202" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D202" t="n">
         <v>9.23501872847885</v>
@@ -10429,13 +10465,13 @@
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B203" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C203" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D203" t="n">
         <v>1.82338253246596</v>
@@ -10464,13 +10500,13 @@
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B204" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C204" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D204" t="n">
         <v>463.861884713451</v>
@@ -10499,13 +10535,13 @@
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B205" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C205" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D205" t="n">
         <v>0.0410579382303959</v>
@@ -10534,13 +10570,13 @@
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B206" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C206" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D206" t="n">
         <v>2.84632344992305</v>
@@ -10569,13 +10605,13 @@
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B207" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C207" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D207" t="n">
         <v>10.4772609490026</v>
@@ -10604,13 +10640,13 @@
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B208" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C208" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D208" t="n">
         <v>7.25547524388075</v>
@@ -10639,13 +10675,13 @@
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B209" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C209" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D209" t="n">
         <v>21.5070584666695</v>
@@ -10674,13 +10710,13 @@
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B210" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C210" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D210" t="n">
         <v>45.6319568374989</v>
@@ -10709,13 +10745,13 @@
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B211" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C211" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D211" t="n">
         <v>3.71488770580898</v>
@@ -10744,13 +10780,13 @@
     </row>
     <row r="212">
       <c r="A212" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B212" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C212" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D212" t="n">
         <v>0</v>
@@ -10779,13 +10815,13 @@
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B213" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C213" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D213" t="n">
         <v>0.0951545653707275</v>
@@ -10814,13 +10850,13 @@
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B214" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C214" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D214" t="n">
         <v>0.260067878955665</v>
@@ -10849,13 +10885,13 @@
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B215" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C215" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D215" t="n">
         <v>0.123302380217443</v>
@@ -10884,13 +10920,13 @@
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B216" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C216" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D216" t="n">
         <v>2.80576191009022</v>
@@ -10919,13 +10955,13 @@
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B217" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C217" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D217" t="n">
         <v>17.9659179544708</v>
@@ -10954,13 +10990,13 @@
     </row>
     <row r="218">
       <c r="A218" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B218" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C218" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D218" t="n">
         <v>0.0050309093813652</v>
@@ -10989,13 +11025,13 @@
     </row>
     <row r="219">
       <c r="A219" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B219" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C219" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D219" t="n">
         <v>29.4582422545772</v>
@@ -11024,13 +11060,13 @@
     </row>
     <row r="220">
       <c r="A220" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B220" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C220" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D220" t="n">
         <v>165.797395991182</v>
@@ -11059,13 +11095,13 @@
     </row>
     <row r="221">
       <c r="A221" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B221" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C221" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D221" t="n">
         <v>0.059388605787885</v>
@@ -11094,13 +11130,13 @@
     </row>
     <row r="222">
       <c r="A222" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B222" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C222" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D222" t="n">
         <v>30.330229117403</v>
@@ -11129,13 +11165,13 @@
     </row>
     <row r="223">
       <c r="A223" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B223" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C223" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D223" t="n">
         <v>330.057950878978</v>
@@ -11164,13 +11200,13 @@
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B224" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C224" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D224" t="n">
         <v>168.599362626556</v>
@@ -11199,13 +11235,13 @@
     </row>
     <row r="225">
       <c r="A225" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B225" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C225" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D225" t="n">
         <v>41.6256809492925</v>
@@ -11234,13 +11270,13 @@
     </row>
     <row r="226">
       <c r="A226" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B226" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C226" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D226" t="n">
         <v>12.4192466361578</v>
@@ -11269,13 +11305,13 @@
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B227" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C227" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D227" t="n">
         <v>49.5275672359959</v>
@@ -11304,13 +11340,13 @@
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B228" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C228" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D228" t="n">
         <v>7.92574001165844</v>
@@ -11339,13 +11375,13 @@
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B229" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C229" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D229" t="n">
         <v>33.3960629193868</v>
@@ -11374,13 +11410,13 @@
     </row>
     <row r="230">
       <c r="A230" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B230" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C230" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D230" t="n">
         <v>29.0120608378559</v>
@@ -11409,13 +11445,13 @@
     </row>
     <row r="231">
       <c r="A231" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B231" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C231" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D231" t="n">
         <v>234.70730505452</v>
@@ -11444,13 +11480,13 @@
     </row>
     <row r="232">
       <c r="A232" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B232" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C232" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D232" t="n">
         <v>63.8580112643012</v>
@@ -11479,13 +11515,13 @@
     </row>
     <row r="233">
       <c r="A233" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B233" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C233" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D233" t="n">
         <v>84.3238204887197</v>
@@ -11514,13 +11550,13 @@
     </row>
     <row r="234">
       <c r="A234" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B234" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C234" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D234" t="n">
         <v>18.1233489687313</v>

</xml_diff>